<commit_message>
Remove separate json files for requests, add posibility to load data from Excel
</commit_message>
<xml_diff>
--- a/TestAutomationFramework/Resource/restApi.xlsx
+++ b/TestAutomationFramework/Resource/restApi.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\JuiceBoxQA\TestAutomationFramework\Resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -932,9 +932,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
Add Json schemas, update requests
</commit_message>
<xml_diff>
--- a/TestAutomationFramework/Resource/restApi.xlsx
+++ b/TestAutomationFramework/Resource/restApi.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="104">
   <si>
     <t>add_unit</t>
   </si>
@@ -365,6 +365,431 @@
 "account_token": "a0c7b2bc-9492-41a3-8124-99e035816550", 
 "token": "7e210d5c773442989d7a122b4442eeca", 
 "device_id": "linker" 
+}</t>
+  </si>
+  <si>
+    <t>{
+    "cmd": "add_car",
+    "account_token": "",
+    "token": "",
+    "device_id": "",
+    "info": {
+        "battery_range_m": 100,
+        "battery_size_wh": 85000,
+        "charging_rate_w": 10000,
+        "description": "2222 Model1s (85 kW-hr battery pack)",
+        "model_id": "66666"
+        }
+}</t>
+  </si>
+  <si>
+    <t>{
+    "cmd": "delete_car",
+    "account_token": "",
+    "token": "",
+    "device_id": "",
+    "info": {
+        "car_id": 0
+        }
+}</t>
+  </si>
+  <si>
+    <t>{
+    "cmd": "update_car",
+    "account_token": "",
+    "token": "",
+    "device_id": "",
+    "info": {
+        "battery_range_m": 0,
+        "car_id": 0,
+        "battery_size_wh": 85000,
+        "charging_rate_w": 10000,
+        "description": "2014 Model1 S (85 kW-hr battery pack)",
+        "model_id": 34775
+        }
+}</t>
+  </si>
+  <si>
+    <t>{
+    "cmd": "select_car",
+    "account_token": "",
+    "token": "",
+    "device_id": "",
+    "info": {
+        "car_id": 0
+        }
+}</t>
+  </si>
+  <si>
+    <t>{
+    "cmd": "add_account_unit",
+    "account_token": "",
+    "device_id": "",
+    "token": ""
+}</t>
+  </si>
+  <si>
+    <t>{
+    "cmd": "add_unit",
+    "device_id": "type anything here",
+    "device_name": "any name",
+    "account_token": "",
+    "ID": "" 
+}</t>
+  </si>
+  <si>
+    <t>{
+    "cmd": "delete_account_unit",
+    "account_token": "",
+    "device_id": "",
+    "token": ""
+}</t>
+  </si>
+  <si>
+    <t>{
+    "cmd": "delete_program_signup_info",
+    "account_token": "",
+    "device_id": "",
+    "token": "",
+    "ID": "string"
+}</t>
+  </si>
+  <si>
+    <t>{
+    "cmd": "get_plot",
+    "device_id": "type anything here",
+    "token": "",
+    "account_token": "",
+    "attribute": "power",
+    "intervals":100,
+    "session_id":5678321
+ }</t>
+  </si>
+  <si>
+    <t>{
+    "cmd": "add_account_unit",
+    "account_token": "a0c7b2bc-9492-41a3-8124-99e035816550",
+    "device_id": "",
+    "token": ""
+}</t>
+  </si>
+  <si>
+    <t>{
+    "cmd": "add_car",
+    "account_token": "a0c7b2bc-9492-41a3-8124-99e035816550",
+    "token": "",
+    "device_id": "",
+    "info": {
+        "battery_range_m": 100,
+        "battery_size_wh": 85000,
+        "charging_rate_w": 10000,
+        "description": "2222 Model1s (85 kW-hr battery pack)",
+        "model_id": "66666"
+        }
+}</t>
+  </si>
+  <si>
+    <t>{
+    "cmd": "add_unit",
+    "device_id": "type anything here",
+    "device_name": "any name",
+    "account_token": "a0c7b2bc-9492-41a3-8124-99e035816550",
+    "ID": "" 
+}</t>
+  </si>
+  <si>
+    <t>{
+    "cmd": "delete_account_unit",
+    "account_token": "a0c7b2bc-9492-41a3-8124-99e035816550",
+    "device_id": "",
+    "token": ""
+}</t>
+  </si>
+  <si>
+    <t>{
+    "cmd": "delete_car",
+    "account_token": "a0c7b2bc-9492-41a3-8124-99e035816550",
+    "token": "",
+    "device_id": "",
+    "info": {
+        "car_id": 0
+        }
+}</t>
+  </si>
+  <si>
+    <t>{
+    "cmd": "delete_program_signup_info",
+    "account_token": "a0c7b2bc-9492-41a3-8124-99e035816550",
+    "device_id": "",
+    "token": "",
+    "ID": "string"
+}</t>
+  </si>
+  <si>
+    <t>{
+    "cmd": "get_plot",
+    "device_id": "type anything here",
+    "token": "",
+    "account_token": "a0c7b2bc-9492-41a3-8124-99e035816550",
+    "attribute": "power",
+    "intervals":100,
+    "session_id":5678321
+ }</t>
+  </si>
+  <si>
+    <t>{
+    "cmd": "select_car",
+    "account_token": "a0c7b2bc-9492-41a3-8124-99e035816550",
+    "token": "",
+    "device_id": "",
+    "info": {
+        "car_id": 0
+        }
+}</t>
+  </si>
+  <si>
+    <t>{
+    "cmd": "update_car",
+    "account_token": "a0c7b2bc-9492-41a3-8124-99e035816550",
+    "token": "",
+    "device_id": "",
+    "info": {
+        "battery_range_m": 0,
+        "car_id": 0,
+        "battery_size_wh": 85000,
+        "charging_rate_w": 10000,
+        "description": "2014 Model1 S (85 kW-hr battery pack)",
+        "model_id": 34775
+        }
+}</t>
+  </si>
+  <si>
+    <t>{
+    "cmd": "get_reset_pin",
+    "ID": "",
+    "device_id": "",
+    "pin": "1234",
+    "step": 0,
+    "session": "string"
+}</t>
+  </si>
+  <si>
+    <t>{
+    "cmd": "get_share_pin",
+    "account_token": "",
+    "device_id": "",
+    "token": ""
+}</t>
+  </si>
+  <si>
+    <t>{
+    "cmd": "logout",
+    "device_id": "",
+    "account_token": ""
+}</t>
+  </si>
+  <si>
+    <t>{
+    "cmd": "pair_device",
+    "device_id": "",
+    "ID": "", 
+    "pin": "1234"
+}</t>
+  </si>
+  <si>
+    <t>{
+    "cmd": "reset_ownership",
+    "account_token": "",
+    "ID": "string",
+    "device_id": "",
+    "step": 0,
+    "session": "string"
+}</t>
+  </si>
+  <si>
+    <t>{
+    "cmd":"set_charging_time",
+    "device_id": "",
+    "token": "",
+    "account_token": "",
+    "charging_time": 1593348596 
+}</t>
+  </si>
+  <si>
+    <t>{
+    "cmd": "register_pushes",
+    "device_id": "",
+    "account_token": "",
+    "push": "string"
+}</t>
+  </si>
+  <si>
+    <t>{
+    "cmd": "set_garage",
+    "account_token": "",
+    "token": "",
+    "device_id": "",
+    "garage_id": "string"
+}</t>
+  </si>
+  <si>
+    <t>{
+    "cmd": "set_info",
+    "account_token": "",
+    "token": "",
+    "device_id": "linker",
+    "name": "EMW Pro 75 JB 3.1 (#7)",
+    "zip": "94070",
+    "country_code": "US",
+    "load_group_id": "string",
+    "unit_type_id": 1,
+    "IP": "50.168.20.98",
+    "gascost": 350,
+    "mpg": 25,
+    "ecost": 12,
+    "whpermile": 300,
+    "timeZoneId": "Pacific Standard Time",
+    "amps_wire_rating": 75,
+    "amps_unit_rating": 75,
+    "info_timestamp": 1499586158,
+    "garage_id": "",
+    "cars": [
+     {
+          "car_id": 5528,
+          "description": "2017 Chevrolet Bolt",
+          "battery_size_wh": 383024,
+          "battery_range_m": 60000,
+          "charging_rate_w": 7200,
+          "model_id": "37066",
+          "model_info": {
+                "model_id": "37066",
+                "description": "2017 Chevrolet Bolt",
+                "make": "Chevrolet",
+                "model": "Bolt",
+                "year": 2017,
+                "range_m": 383023,
+                "range_city_m": 399116,
+                "range_highway_m": 337961,
+                "battery_size_wh": 60000,
+                "charging_rate_w": 7200,
+                "images": {
+                    "charging": "string",
+                    "default": "https://dashboard.emotorwerks.com/Content/carmodels/chevy_bolt.jpg",
+                    "plugged": "string"
+                }
+            }
+         }
+  ],
+    "policy": {
+            "name": "string",
+            "user_control_allowed": false,
+            "charge_control_type": "string"
+        }
+}</t>
+  </si>
+  <si>
+    <t>{
+    "cmd":"set_limit",
+    "device_id":"",
+    "token":"",
+    "amperage": 15
+}</t>
+  </si>
+  <si>
+    <t>{
+  "cmd": "set_notifications",
+  "token": "string",
+  "device_id": "string",
+  "charging_delayed_due_to_ToU": {
+ "email": true,
+ "push": true
+  },
+  "start_charging": {
+ "email": true,
+ "push": true
+  },
+  "stop_charging": {
+ "email": true,
+ "push": true
+  },
+  "is_offline": {
+ "email": true,
+ "push": true
+  },
+  "is_back_online": {
+ "email": true,
+ "push": true
+  },
+  "is_not_plugged_in_by": {
+ "email": true,
+ "push": true,
+ "time": 0
+  }
+}</t>
+  </si>
+  <si>
+    <t>{
+    "cmd": "“set_override"”,
+    "account_token": "",
+    "token": "",
+    "device_id": "",
+    "energy_at_plugin": 0,
+    "override_time": 156262626,
+    "energy_to_add": 40000
+}</t>
+  </si>
+  <si>
+    <t>{ 
+    "cmd": "set_program_signup_info",
+    "token": "",
+    "device_id": "",
+    "userinfo": {
+              "first_name": "Andriy",
+             "last_name": "Fedorenko",
+             "name_is_different_in_bill": "",
+             "bill_first_name": "Andriy",
+             "bill_last_name": "Fedorenko",
+             "email": "ANnnndriy@emotorwerks.com",
+             "phone_number": "4154568956",
+             "address": "linekr idet domioi",
+             "city": "cool stuff",
+             "service_address": "ninto ne znaet",
+             "service_city": "San Carol",
+             "state": "Null",
+             "post_code": "95128",
+             "images": [
+                        "string"
+              ]
+         }
+ }</t>
+  </si>
+  <si>
+    <t>{
+    "cmd":"set_schedule",
+    "device_id":"",
+    "token":"",
+    "type": "custom",
+    "account_token":"",
+    "weekday": {
+        "start": 1380,
+        "end": 420,
+        "car_ready_by": 0
+    },
+    "weekend": {
+        "start": 1380,
+        "end": 480,
+        "car_ready_by": 0
+    }
+}</t>
+  </si>
+  <si>
+    <t>{
+    "cmd": "share_device",
+    "device_id": "",
+    "device_name": "string",
+    "account_token": "",
+    "ID": "",
+    "pin": "1235"
 }</t>
   </si>
 </sst>
@@ -404,7 +829,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -426,6 +851,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -605,7 +1036,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -648,6 +1079,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -932,7 +1369,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
@@ -955,29 +1394,47 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="87" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="9"/>
-    </row>
-    <row r="3" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+      <c r="B2" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="188.5" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="9"/>
-    </row>
-    <row r="4" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+      <c r="B3" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="101.5" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="9"/>
+      <c r="B4" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="58" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
@@ -993,29 +1450,47 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="87" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="9"/>
-    </row>
-    <row r="7" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+      <c r="B6" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="130.5" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="9"/>
-    </row>
-    <row r="8" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+      <c r="B7" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="101.5" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="9"/>
+      <c r="B8" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="9" spans="1:4" ht="72.5" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
@@ -1087,13 +1562,19 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="130.5" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9"/>
+      <c r="B14" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="15" spans="1:4" ht="87" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
@@ -1109,13 +1590,19 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="116" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="15"/>
+      <c r="B16" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="17" spans="1:4" ht="87" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
@@ -1145,13 +1632,19 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="87" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="9"/>
+      <c r="B19" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="20" spans="1:4" ht="87" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
@@ -1195,125 +1688,215 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="72.5" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="9"/>
-    </row>
-    <row r="24" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+      <c r="B23" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="87" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="9"/>
-    </row>
-    <row r="25" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+      <c r="B24" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="87" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="9"/>
-    </row>
-    <row r="26" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+      <c r="B25" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="116" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="9"/>
-    </row>
-    <row r="27" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+      <c r="B26" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="130.5" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="9"/>
-    </row>
-    <row r="28" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+      <c r="B27" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="101.5" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="9"/>
-    </row>
-    <row r="29" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+      <c r="B28" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="101.5" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="9"/>
-    </row>
-    <row r="30" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+      <c r="B29" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="9"/>
-    </row>
-    <row r="31" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+      <c r="B30" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="87" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="9"/>
-    </row>
-    <row r="32" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+      <c r="B31" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="9"/>
-    </row>
-    <row r="33" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+      <c r="B32" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="130.5" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="9"/>
-    </row>
-    <row r="34" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+      <c r="B33" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="333.5" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="9"/>
-    </row>
-    <row r="35" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+      <c r="B34" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="246.5" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="9"/>
-    </row>
-    <row r="36" spans="1:4" ht="14.5" x14ac:dyDescent="0.3">
+      <c r="B35" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="116" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="9"/>
-    </row>
-    <row r="37" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="203.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B37" s="12"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="13"/>
+      <c r="B37" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="D37" s="13" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="38" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="2"/>

</xml_diff>

<commit_message>
Modify Api test functionalyty. Add possibility to pass parameters from feature file
</commit_message>
<xml_diff>
--- a/TestAutomationFramework/Resource/restApi.xlsx
+++ b/TestAutomationFramework/Resource/restApi.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="105">
   <si>
     <t>add_unit</t>
   </si>
@@ -156,13 +156,6 @@
     <t>{
 "cmd": "check_device",
 "ID": "373769600"
-}</t>
-  </si>
-  <si>
-    <t>{
-"cmd": "get_account_units",
-"device_id": "linker",
-"account_token": "a0c7b2bc-9492-41a3-8124-99e035816550"
 }</t>
   </si>
   <si>
@@ -309,62 +302,6 @@
 "account_token": "7dc4abd2-5b51-4c02-9c16-fc4d7f816366",
 "token": "c61f3ed4a0ee496589a533d6977f86bb",
 "device_id": "linker"
-}</t>
-  </si>
-  <si>
-    <t>{
-"cmd": "get_history",
-"account_token": "a0c7b2bc-9492-41a3-8124-99e035816550",
-"token": "7e210d5c773442989d7a122b4442eeca",
-"device_id": "linker"
-}</t>
-  </si>
-  <si>
-    <t>{ 
-"cmd": "get_info", 
-"account_token": "a0c7b2bc-9492-41a3-8124-99e035816550", 
-"token": "7e210d5c773442989d7a122b4442eeca", 
-"device_id": "linker" 
-}</t>
-  </si>
-  <si>
-    <t>{ 
-"cmd": "get_notifications", 
-"account_token": "a0c7b2bc-9492-41a3-8124-99e035816550", 
-"token": "7e210d5c773442989d7a122b4442eeca", 
-"device_id": "linker" 
-}</t>
-  </si>
-  <si>
-    <t>{ 
-"cmd": "get_program_signup_info", 
-"account_token": "a0c7b2bc-9492-41a3-8124-99e035816550", 
-"token": "7e210d5c773442989d7a122b4442eeca", 
-"device_id": "linker" 
-}</t>
-  </si>
-  <si>
-    <t>{ 
-"cmd": "get_schedule", 
-"account_token": "a0c7b2bc-9492-41a3-8124-99e035816550", 
-"token": "7e210d5c773442989d7a122b4442eeca", 
-"device_id": "linker" 
-}</t>
-  </si>
-  <si>
-    <t>{ 
-"cmd": "get_state", 
-"account_token": "a0c7b2bc-9492-41a3-8124-99e035816550", 
-"token": "7e210d5c773442989d7a122b4442eeca", 
-"device_id": "linker" 
-}</t>
-  </si>
-  <si>
-    <t>{ 
-"cmd": "get_utilitybill_url", 
-"account_token": "a0c7b2bc-9492-41a3-8124-99e035816550", 
-"token": "7e210d5c773442989d7a122b4442eeca", 
-"device_id": "linker" 
 }</t>
   </si>
   <si>
@@ -790,6 +727,124 @@
     "account_token": "",
     "ID": "",
     "pin": "1235"
+}</t>
+  </si>
+  <si>
+    <t>{
+"cmd": "get_account_units",
+"device_id": "Test device",
+"account_token": "a0c7b2bc-9492-41a3-8124-99e035816550"
+}</t>
+  </si>
+  <si>
+    <t>{
+"cmd": "get_history",
+"account_token": "a0c7b2bc-9492-41a3-8124-99e035816550",
+"token": "3ffbf508342447a788f5380ab382f57f",
+"device_id": "Test device"
+}</t>
+  </si>
+  <si>
+    <t>{ 
+"cmd": "get_info", 
+"account_token": "a0c7b2bc-9492-41a3-8124-99e035816550", 
+"token": "3ffbf508342447a788f5380ab382f57f", 
+"device_id": "Test device" 
+}</t>
+  </si>
+  <si>
+    <t>{ 
+"cmd": "get_notifications", 
+"account_token": "a0c7b2bc-9492-41a3-8124-99e035816550", 
+"token": "3ffbf508342447a788f5380ab382f57f", 
+"device_id": "Test device" 
+}</t>
+  </si>
+  <si>
+    <t>{ 
+"cmd": "get_program_signup_info", 
+"account_token": "a0c7b2bc-9492-41a3-8124-99e035816550", 
+"token": "3ffbf508342447a788f5380ab382f57f", 
+"device_id": "Test device" 
+}</t>
+  </si>
+  <si>
+    <t>{ 
+"cmd": "get_schedule", 
+"account_token": "a0c7b2bc-9492-41a3-8124-99e035816550", 
+"token": "3ffbf508342447a788f5380ab382f57f", 
+"device_id": "Test device" 
+}</t>
+  </si>
+  <si>
+    <t>{ 
+"cmd": "get_state", 
+"account_token": "a0c7b2bc-9492-41a3-8124-99e035816550", 
+"token": "3ffbf508342447a788f5380ab382f57f", 
+"device_id": "Test device" 
+}</t>
+  </si>
+  <si>
+    <t>{ 
+"cmd": "get_utilitybill_url", 
+"account_token": "a0c7b2bc-9492-41a3-8124-99e035816550", 
+"token": "3ffbf508342447a788f5380ab382f57f", 
+"device_id": "Test device" 
+}</t>
+  </si>
+  <si>
+    <t>{
+    "cmd": "set_info",
+    "account_token": "",
+    "token": "",
+    "device_id": "Test device",
+    "name": "EMW Pro 75 JB 3.1 (#7)",
+    "zip": "94070",
+    "country_code": "US",
+    "load_group_id": "string",
+    "unit_type_id": 1,
+    "IP": "50.168.20.98",
+    "gascost": 350,
+    "mpg": 25,
+    "ecost": 12,
+    "whpermile": 300,
+    "timeZoneId": "Pacific Standard Time",
+    "amps_wire_rating": 75,
+    "amps_unit_rating": 75,
+    "info_timestamp": 1499586158,
+    "garage_id": "",
+    "cars": [
+     {
+          "car_id": 5528,
+          "description": "2017 Chevrolet Bolt",
+          "battery_size_wh": 383024,
+          "battery_range_m": 60000,
+          "charging_rate_w": 7200,
+          "model_id": "37066",
+          "model_info": {
+                "model_id": "37066",
+                "description": "2017 Chevrolet Bolt",
+                "make": "Chevrolet",
+                "model": "Bolt",
+                "year": 2017,
+                "range_m": 383023,
+                "range_city_m": 399116,
+                "range_highway_m": 337961,
+                "battery_size_wh": 60000,
+                "charging_rate_w": 7200,
+                "images": {
+                    "charging": "string",
+                    "default": "https://dashboard.emotorwerks.com/Content/carmodels/chevy_bolt.jpg",
+                    "plugged": "string"
+                }
+            }
+         }
+  ],
+    "policy": {
+            "name": "string",
+            "user_control_allowed": false,
+            "charge_control_type": "string"
+        }
 }</t>
   </si>
 </sst>
@@ -1369,8 +1424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B11" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1399,13 +1454,13 @@
         <v>11</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="188.5" x14ac:dyDescent="0.3">
@@ -1413,13 +1468,13 @@
         <v>12</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="101.5" x14ac:dyDescent="0.3">
@@ -1427,13 +1482,13 @@
         <v>0</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="58" x14ac:dyDescent="0.3">
@@ -1455,13 +1510,13 @@
         <v>14</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="130.5" x14ac:dyDescent="0.3">
@@ -1469,13 +1524,13 @@
         <v>15</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="101.5" x14ac:dyDescent="0.3">
@@ -1483,13 +1538,13 @@
         <v>16</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="72.5" x14ac:dyDescent="0.3">
@@ -1497,13 +1552,13 @@
         <v>1</v>
       </c>
       <c r="B9" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="D9" s="15" t="s">
         <v>44</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="43.5" x14ac:dyDescent="0.3">
@@ -1511,13 +1566,13 @@
         <v>17</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="87" x14ac:dyDescent="0.3">
@@ -1525,13 +1580,13 @@
         <v>6</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>64</v>
+        <v>97</v>
       </c>
       <c r="C11" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="15" t="s">
         <v>47</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="87" x14ac:dyDescent="0.3">
@@ -1539,13 +1594,13 @@
         <v>18</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="C12" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="15" t="s">
         <v>49</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="87" x14ac:dyDescent="0.3">
@@ -1553,13 +1608,13 @@
         <v>19</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>66</v>
+        <v>99</v>
       </c>
       <c r="C13" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="15" t="s">
         <v>51</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="130.5" x14ac:dyDescent="0.3">
@@ -1567,13 +1622,13 @@
         <v>20</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="87" x14ac:dyDescent="0.3">
@@ -1581,13 +1636,13 @@
         <v>21</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>67</v>
+        <v>100</v>
       </c>
       <c r="C15" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" s="15" t="s">
         <v>53</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="116" x14ac:dyDescent="0.3">
@@ -1595,13 +1650,13 @@
         <v>22</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="87" x14ac:dyDescent="0.3">
@@ -1609,13 +1664,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
       <c r="C17" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="15" t="s">
         <v>55</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="43.5" x14ac:dyDescent="0.3">
@@ -1623,13 +1678,13 @@
         <v>23</v>
       </c>
       <c r="B18" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="15" t="s">
         <v>57</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="87" x14ac:dyDescent="0.3">
@@ -1637,13 +1692,13 @@
         <v>24</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="87" x14ac:dyDescent="0.3">
@@ -1651,13 +1706,13 @@
         <v>2</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>69</v>
+        <v>102</v>
       </c>
       <c r="C20" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="15" t="s">
         <v>59</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="43.5" x14ac:dyDescent="0.3">
@@ -1665,13 +1720,13 @@
         <v>25</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="87" x14ac:dyDescent="0.3">
@@ -1679,13 +1734,13 @@
         <v>26</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>70</v>
+        <v>103</v>
       </c>
       <c r="C22" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" s="15" t="s">
         <v>62</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="72.5" x14ac:dyDescent="0.3">
@@ -1693,13 +1748,13 @@
         <v>27</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="87" x14ac:dyDescent="0.3">
@@ -1707,13 +1762,13 @@
         <v>28</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="87" x14ac:dyDescent="0.3">
@@ -1721,13 +1776,13 @@
         <v>29</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="116" x14ac:dyDescent="0.3">
@@ -1735,13 +1790,13 @@
         <v>30</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="130.5" x14ac:dyDescent="0.3">
@@ -1749,13 +1804,13 @@
         <v>31</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="101.5" x14ac:dyDescent="0.3">
@@ -1763,13 +1818,13 @@
         <v>32</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="101.5" x14ac:dyDescent="0.3">
@@ -1777,13 +1832,13 @@
         <v>33</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="409.5" x14ac:dyDescent="0.3">
@@ -1791,13 +1846,13 @@
         <v>34</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="87" x14ac:dyDescent="0.3">
@@ -1805,13 +1860,13 @@
         <v>3</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="409.5" x14ac:dyDescent="0.3">
@@ -1819,13 +1874,13 @@
         <v>35</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="130.5" x14ac:dyDescent="0.3">
@@ -1833,13 +1888,13 @@
         <v>36</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="333.5" x14ac:dyDescent="0.3">
@@ -1847,13 +1902,13 @@
         <v>37</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="246.5" x14ac:dyDescent="0.3">
@@ -1861,13 +1916,13 @@
         <v>5</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="116" x14ac:dyDescent="0.3">
@@ -1875,13 +1930,13 @@
         <v>38</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="203.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -1889,13 +1944,13 @@
         <v>39</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="D37" s="13" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>